<commit_message>
change intro and planeación
</commit_message>
<xml_diff>
--- a/docs/_static/FormatoPlaneacionSimulacion2023-10.xlsx
+++ b/docs/_static/FormatoPlaneacionSimulacion2023-10.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E828863B-001B-40F2-99D9-C5F97AE196CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84275A31-F69A-4D81-9E40-7256101BF754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,21 @@
     <definedName name="AMPLIONBC">[1]Listas!$H$2:$H$11</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Proyecto Docente'!$A$1:$M$31</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -109,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
   <si>
     <t>PROYECTO DOCENTE</t>
   </si>
@@ -331,15 +342,6 @@
     <t>En el sitio están las fechas, secuencias de actividades y evaluación. Con la evaluación se verificará la lectura del sitio</t>
   </si>
   <si>
-    <t>Presentación del curso, motivación y sentido</t>
-  </si>
-  <si>
-    <t>Sitio web del curso. Internet</t>
-  </si>
-  <si>
-    <t>Formativa</t>
-  </si>
-  <si>
     <t>Texto guía y sitio web del curso</t>
   </si>
   <si>
@@ -361,54 +363,65 @@
     <t>Sistemas de partículas</t>
   </si>
   <si>
-    <t>Componentes físicos</t>
-  </si>
-  <si>
     <t>Agentes autónomos</t>
   </si>
   <si>
-    <t>Fractales</t>
-  </si>
-  <si>
-    <t>Algortitmos evalutivos</t>
-  </si>
-  <si>
-    <t>Redes neuronales</t>
-  </si>
-  <si>
-    <t>Trabajo Final</t>
-  </si>
-  <si>
-    <t>1 h 40 min Presentación del curso y motivación</t>
-  </si>
-  <si>
-    <t>1 h 40 min. Presentaciones de cada estudiante</t>
-  </si>
-  <si>
-    <t>1 h 40 min. Presentación y evaluación de trabajos finales. 
-2 horas. Evaluación del curso y mejoras para 2023-20</t>
-  </si>
-  <si>
-    <t>3 h 20 min para trabajar en clase, mostrar avances de la sesión presencial y autónoma y resolver dudas</t>
-  </si>
-  <si>
-    <t>3 h 20 min. Realización y sustentación de los ejercicios y retos</t>
-  </si>
-  <si>
-    <t>2 h. Repositorio con los referentes encontrados y preparación de una presentación de 5 minutos de los referentes</t>
-  </si>
-  <si>
-    <t>2 h. Lectura del capítulo correspondiente del texto guía</t>
-  </si>
-  <si>
-    <t>2 h. Continuación del trabajo final</t>
+    <t>Componentes Físicos</t>
+  </si>
+  <si>
+    <t>1 h 40 min presentación del curso</t>
+  </si>
+  <si>
+    <t>1 h 40 min. Lectura y ejercicios</t>
+  </si>
+  <si>
+    <t>2 h. Lectura y ejercicios</t>
+  </si>
+  <si>
+    <t>3 h 20 min. Lectura, ejercicios y paso 1 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>3 h 20 min. Lectura y ejercicios</t>
+  </si>
+  <si>
+    <t>2 h. Lectura, ejercicios, paso 1 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>3 h 20 min. Lectura, ejercicios y paso 2 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>2 h. Lectura, ejercicios, paso 2 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>3 h 20 min. Lectura, ejercicios y paso 3 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>2 h. Lectura, ejercicios, paso 3 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>3 h 20 min. Lectura, ejercicios y paso 4 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>2 h. Lectura, ejercicios, paso 4 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>3 h 20 min. Lectura, ejercicios y paso 5 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>2 h. Lectura, ejercicios, paso 5 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>3 h 20 min. Lectura, ejercicios y paso 6 del proyecto de curso</t>
+  </si>
+  <si>
+    <t>2 h. Lectura, ejercicios, paso 6 del proyecto de curso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +507,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1167,7 +1187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1219,18 +1239,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1243,6 +1254,156 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1252,18 +1413,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1312,12 +1461,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1342,143 +1485,23 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1899,8 +1922,8 @@
   </sheetPr>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="30" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:M6"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" zoomScalePageLayoutView="30" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1909,9 +1932,9 @@
     <col min="2" max="2" width="16.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="30" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.26953125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" customWidth="1"/>
     <col min="8" max="8" width="26" style="3" customWidth="1"/>
     <col min="9" max="9" width="18.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.26953125" style="1" customWidth="1"/>
@@ -1923,159 +1946,159 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29.25" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="83"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="40"/>
     </row>
     <row r="2" spans="1:13" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="86"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
     </row>
     <row r="3" spans="1:13" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="88"/>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="89"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="90"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="91"/>
-      <c r="I4" s="91"/>
-      <c r="J4" s="91"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="93"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="50"/>
     </row>
     <row r="5" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="94"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="97"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="54"/>
     </row>
     <row r="6" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="B6" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="62"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="65"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="58"/>
     </row>
     <row r="7" spans="1:13" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="66">
+      <c r="B7" s="59">
         <v>11443</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="68"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="62"/>
     </row>
     <row r="8" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="70">
         <v>2</v>
       </c>
-      <c r="C8" s="53"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="7">
         <v>96</v>
       </c>
-      <c r="F8" s="80" t="s">
+      <c r="F8" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="80"/>
+      <c r="G8" s="75"/>
       <c r="H8" s="7">
         <v>64</v>
       </c>
-      <c r="I8" s="77" t="s">
+      <c r="I8" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-      <c r="L8" s="79"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="74"/>
       <c r="M8" s="8">
         <v>32</v>
       </c>
@@ -2084,20 +2107,20 @@
       <c r="A9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="73"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="66"/>
     </row>
     <row r="10" spans="1:13" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
@@ -2107,52 +2130,52 @@
         <v>43</v>
       </c>
       <c r="C10" s="10"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="75"/>
-      <c r="L10" s="75"/>
-      <c r="M10" s="76"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="69"/>
     </row>
     <row r="11" spans="1:13" s="4" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="102" t="s">
+      <c r="D11" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="34" t="s">
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="100" t="s">
+      <c r="K11" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="34" t="s">
+      <c r="L11" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="M11" s="34" t="s">
+      <c r="M11" s="28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="105"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="33"/>
+    <row r="12" spans="1:13" s="4" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="35"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="104"/>
       <c r="D12" s="18" t="s">
         <v>5</v>
       </c>
@@ -2171,467 +2194,425 @@
       <c r="I12" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="35"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-    </row>
-    <row r="13" spans="1:13" ht="62.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="106"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+    </row>
+    <row r="13" spans="1:13" ht="55" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
       <c r="B13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" s="2"/>
+      <c r="C13" s="105" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="I13" s="15"/>
       <c r="J13" s="2" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="M13" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A14" s="106"/>
+        <v>61</v>
+      </c>
+      <c r="L13" s="2"/>
+      <c r="M13" s="21"/>
+    </row>
+    <row r="14" spans="1:13" ht="52" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>66</v>
-      </c>
+      <c r="C14" s="106"/>
       <c r="D14" s="5"/>
       <c r="E14" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="15"/>
+      <c r="I14" s="2"/>
       <c r="J14" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M14" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A15" s="106"/>
+        <v>62</v>
+      </c>
+      <c r="M14" s="21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>67</v>
+      <c r="C15" s="105" t="s">
+        <v>64</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="2"/>
+      <c r="I15" s="15"/>
       <c r="J15" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M15" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A16" s="106"/>
+        <v>61</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="21"/>
+    </row>
+    <row r="16" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="C16" s="106"/>
       <c r="D16" s="5"/>
       <c r="E16" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="6"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A17" s="106"/>
+        <v>62</v>
+      </c>
+      <c r="M16" s="21">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
       <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>69</v>
+      <c r="C17" s="105" t="s">
+        <v>65</v>
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="6"/>
-      <c r="I17" s="2"/>
+      <c r="I17" s="15"/>
       <c r="J17" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M17" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A18" s="106"/>
+        <v>61</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="21"/>
+    </row>
+    <row r="18" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
       <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>70</v>
-      </c>
+      <c r="C18" s="106"/>
       <c r="D18" s="5"/>
       <c r="E18" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="6"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M18" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A19" s="106"/>
+        <v>62</v>
+      </c>
+      <c r="M18" s="21">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
       <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>71</v>
+      <c r="C19" s="105" t="s">
+        <v>66</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="2"/>
+      <c r="I19" s="15"/>
       <c r="J19" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M19" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A20" s="106"/>
+        <v>61</v>
+      </c>
+      <c r="L19" s="2"/>
+      <c r="M19" s="21"/>
+    </row>
+    <row r="20" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
       <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>72</v>
-      </c>
+      <c r="C20" s="107"/>
       <c r="D20" s="5"/>
       <c r="E20" s="2" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="2"/>
+      <c r="I20" s="15"/>
       <c r="J20" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L20" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M20" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A21" s="106"/>
+        <v>61</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="21"/>
+    </row>
+    <row r="21" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
       <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="C21" s="106"/>
       <c r="D21" s="5"/>
       <c r="E21" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="6"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M21" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A22" s="106"/>
+        <v>62</v>
+      </c>
+      <c r="M21" s="21">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="108"/>
+      <c r="E22" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="2"/>
+      <c r="I22" s="15"/>
       <c r="J22" s="2" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M22" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="50" x14ac:dyDescent="0.25">
-      <c r="A23" s="106"/>
+        <v>61</v>
+      </c>
+      <c r="L22" s="2"/>
+      <c r="M22" s="21"/>
+    </row>
+    <row r="23" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
       <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="5"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="108"/>
       <c r="E23" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="6"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L23" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M23" s="22">
-        <v>7.0000000000000007E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="106"/>
+        <v>62</v>
+      </c>
+      <c r="M23" s="21">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="2"/>
+      <c r="C24" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="D24" s="108"/>
+      <c r="E24" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F24" s="2"/>
-      <c r="G24" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="G24" s="2"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="2"/>
+      <c r="I24" s="15"/>
       <c r="J24" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M24" s="23">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="106"/>
+        <v>72</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L24" s="2"/>
+      <c r="M24" s="21"/>
+    </row>
+    <row r="25" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
       <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="108"/>
+      <c r="E25" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="F25" s="2"/>
-      <c r="G25" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="G25" s="2"/>
       <c r="H25" s="6"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K25" s="2"/>
+        <v>83</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="L25" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M25" s="23">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="106"/>
+        <v>62</v>
+      </c>
+      <c r="M25" s="21">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
       <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>76</v>
+      <c r="C26" s="105" t="s">
+        <v>68</v>
       </c>
       <c r="D26" s="5"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="G26" s="2"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="2"/>
+      <c r="I26" s="15"/>
       <c r="J26" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M26" s="23">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="106"/>
+        <v>72</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="21"/>
+    </row>
+    <row r="27" spans="1:13" ht="25" x14ac:dyDescent="0.25">
+      <c r="A27" s="36"/>
       <c r="B27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>76</v>
-      </c>
+      <c r="C27" s="107"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F27" s="2"/>
-      <c r="G27" s="2" t="s">
-        <v>80</v>
-      </c>
+      <c r="G27" s="2"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="2"/>
+      <c r="I27" s="15"/>
       <c r="J27" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M27" s="23">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="106"/>
+        <v>72</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="21"/>
+    </row>
+    <row r="28" spans="1:13" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
       <c r="B28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>76</v>
-      </c>
+      <c r="C28" s="106"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>84</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="L28" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M28" s="22">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="106"/>
+        <v>62</v>
+      </c>
+      <c r="M28" s="21">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="36"/>
       <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
@@ -2645,10 +2626,13 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="24"/>
+      <c r="M29" s="21">
+        <f>SUM(M13:M28)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="106"/>
+      <c r="A30" s="36"/>
       <c r="B30" s="5" t="s">
         <v>28</v>
       </c>
@@ -2662,202 +2646,193 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="24"/>
+      <c r="M30" s="21"/>
     </row>
     <row r="31" spans="1:13" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="107"/>
-      <c r="B31" s="25" t="s">
+      <c r="A31" s="37"/>
+      <c r="B31" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="27"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="28"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="25"/>
     </row>
     <row r="32" spans="1:13" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="35" t="s">
+      <c r="A32" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="86" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="44"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="45"/>
+      <c r="C32" s="87"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="87"/>
+      <c r="F32" s="87"/>
+      <c r="G32" s="87"/>
+      <c r="H32" s="88"/>
       <c r="I32" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J32" s="39" t="s">
+      <c r="J32" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="K32" s="40"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="41"/>
+      <c r="K32" s="83"/>
+      <c r="L32" s="83"/>
+      <c r="M32" s="84"/>
     </row>
     <row r="33" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="46" t="s">
+      <c r="A33" s="29"/>
+      <c r="B33" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="47"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="48"/>
+      <c r="C33" s="90"/>
+      <c r="D33" s="90"/>
+      <c r="E33" s="90"/>
+      <c r="F33" s="90"/>
+      <c r="G33" s="90"/>
+      <c r="H33" s="91"/>
       <c r="I33" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="J33" s="56" t="s">
+      <c r="J33" s="97" t="s">
         <v>57</v>
       </c>
-      <c r="K33" s="57"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="58"/>
+      <c r="K33" s="98"/>
+      <c r="L33" s="98"/>
+      <c r="M33" s="99"/>
     </row>
     <row r="34" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35"/>
-      <c r="B34" s="49" t="s">
+      <c r="A34" s="29"/>
+      <c r="B34" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="51"/>
+      <c r="C34" s="93"/>
+      <c r="D34" s="93"/>
+      <c r="E34" s="93"/>
+      <c r="F34" s="93"/>
+      <c r="G34" s="93"/>
+      <c r="H34" s="94"/>
       <c r="I34" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="J34" s="59" t="s">
+      <c r="J34" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="K34" s="60"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="61"/>
+      <c r="K34" s="101"/>
+      <c r="L34" s="101"/>
+      <c r="M34" s="102"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="53"/>
+      <c r="A35" s="29"/>
+      <c r="B35" s="70"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="71"/>
       <c r="I35" s="15"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="31"/>
+      <c r="J35" s="76"/>
+      <c r="K35" s="77"/>
+      <c r="L35" s="77"/>
+      <c r="M35" s="78"/>
     </row>
     <row r="36" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="35"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="53"/>
+      <c r="A36" s="29"/>
+      <c r="B36" s="70"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="77"/>
+      <c r="E36" s="77"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="77"/>
+      <c r="H36" s="71"/>
       <c r="I36" s="15"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="31"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="77"/>
+      <c r="L36" s="77"/>
+      <c r="M36" s="78"/>
     </row>
     <row r="37" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="35"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="53"/>
+      <c r="A37" s="29"/>
+      <c r="B37" s="70"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="77"/>
+      <c r="G37" s="77"/>
+      <c r="H37" s="71"/>
       <c r="I37" s="15"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="31"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="77"/>
+      <c r="L37" s="77"/>
+      <c r="M37" s="78"/>
     </row>
     <row r="38" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="53"/>
+      <c r="A38" s="29"/>
+      <c r="B38" s="70"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="77"/>
+      <c r="G38" s="77"/>
+      <c r="H38" s="71"/>
       <c r="I38" s="15"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="31"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="77"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="78"/>
     </row>
     <row r="39" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="53"/>
+      <c r="A39" s="29"/>
+      <c r="B39" s="70"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="77"/>
+      <c r="G39" s="77"/>
+      <c r="H39" s="71"/>
       <c r="I39" s="15"/>
-      <c r="J39" s="29"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="31"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="77"/>
+      <c r="L39" s="77"/>
+      <c r="M39" s="78"/>
     </row>
     <row r="40" spans="1:13" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="42"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="55"/>
+      <c r="A40" s="85"/>
+      <c r="B40" s="95"/>
+      <c r="C40" s="80"/>
+      <c r="D40" s="80"/>
+      <c r="E40" s="80"/>
+      <c r="F40" s="80"/>
+      <c r="G40" s="80"/>
+      <c r="H40" s="96"/>
       <c r="I40" s="16"/>
-      <c r="J40" s="36"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="37"/>
-      <c r="M40" s="38"/>
+      <c r="J40" s="79"/>
+      <c r="K40" s="80"/>
+      <c r="L40" s="80"/>
+      <c r="M40" s="81"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="A13:C14 I12 I11:J11 D11:H14 L11 A11:C11 K11:K12 J14 K13:M14 I13:J13 A15:M31" name="Rango1"/>
+    <protectedRange sqref="I12 I11:J11 C13:H13 L11 A11:C11 K11:K12 J13:M13 C15:H15 C19:D21 A30:M31 D11:H12 A13:B29 C29:M29 C14:M14 C16:M16 J15:M15 C17:H17 C18:M18 J17:M17 K19:M21 E21:J21 E19:H20 J19:J20 C23:M23 C22:H22 J22:M22 E25:J25 E24:H24 J24 C24:D28 K24:M28 E28:J28 E26:H27 J26:J27" name="Rango1"/>
   </protectedRanges>
-  <mergeCells count="39">
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="D11:I11"/>
-    <mergeCell ref="A11:A31"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="B4:M4"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B6:M6"/>
-    <mergeCell ref="B7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="D10:M10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="F8:G8"/>
+  <mergeCells count="46">
+    <mergeCell ref="J35:M35"/>
+    <mergeCell ref="J36:M36"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C26:C28"/>
     <mergeCell ref="J38:M38"/>
     <mergeCell ref="J39:M39"/>
     <mergeCell ref="J40:M40"/>
@@ -2874,15 +2849,31 @@
     <mergeCell ref="B40:H40"/>
     <mergeCell ref="J33:M33"/>
     <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J35:M35"/>
-    <mergeCell ref="J36:M36"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="B6:M6"/>
+    <mergeCell ref="B7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="D10:M10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="I8:L8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="B4:M4"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="A11:A31"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10:C10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Presencial, virtual, bimodal, a distancia, dual"</formula1>
     </dataValidation>
@@ -2901,25 +2892,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_activity xmlns="475903d6-5b88-4d7a-ba78-d123e191ef42" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010007385DC504DB614DA8F67D4315A28B14" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3ac3543c8bd13c0fc9dcbaaaa4f4e21f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="1be38a3c-13c4-46e0-8a29-91f320e906cc" xmlns:ns4="475903d6-5b88-4d7a-ba78-d123e191ef42" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="832580f857820fba5b25e66e4b08a8f5" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3177,33 +3149,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDE66BE-7C4D-4D57-9569-773F449FD84D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1be38a3c-13c4-46e0-8a29-91f320e906cc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="475903d6-5b88-4d7a-ba78-d123e191ef42"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635976DF-2941-4508-B3B6-F1CF25643BD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_activity xmlns="475903d6-5b88-4d7a-ba78-d123e191ef42" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0C325370-FB0B-42DC-B685-563E2C80434A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3221,4 +3186,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{635976DF-2941-4508-B3B6-F1CF25643BD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDE66BE-7C4D-4D57-9569-773F449FD84D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1be38a3c-13c4-46e0-8a29-91f320e906cc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="475903d6-5b88-4d7a-ba78-d123e191ef42"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>